<commit_message>
Move analog muxes to analog power domain
</commit_message>
<xml_diff>
--- a/AD5933_BOM2.xlsx
+++ b/AD5933_BOM2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athul_AT\Documents\eagle\AD5933\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Athul_AT\Documents\eagle\AD5933_board\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>